<commit_message>
Test Cases from DAO
</commit_message>
<xml_diff>
--- a/src/test/resources/OpenWeatherMapTestCases.xlsx
+++ b/src/test/resources/OpenWeatherMapTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ByCityName" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="36">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -95,6 +95,36 @@
   </si>
   <si>
     <t>INVALID_DATA</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>Valid Geo Coords</t>
+  </si>
+  <si>
+    <t>Invalid Geo Coords</t>
+  </si>
+  <si>
+    <t>Country Code</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>Mountain View</t>
+  </si>
+  <si>
+    <t>XXXXX</t>
+  </si>
+  <si>
+    <t>ZZ</t>
   </si>
 </sst>
 </file>
@@ -580,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,24 +736,264 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>-16.920000000000002</v>
+      </c>
+      <c r="E2">
+        <v>145.77000000000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>200</v>
+      </c>
+      <c r="L2">
+        <v>2172797</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>3002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>360</v>
+      </c>
+      <c r="E3">
+        <v>-1000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3">
+        <v>404</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>94040</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>200</v>
+      </c>
+      <c r="L2">
+        <v>5375480</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>3002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3">
+        <v>404</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>